<commit_message>
Affichage recette, modification recette, delete recette
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="A3:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,17 +530,17 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -561,47 +561,47 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -622,7 +622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>